<commit_message>
-documentation update -XML added
</commit_message>
<xml_diff>
--- a/PlexByte.App.MoCap.Docs/Code Dockumentation fabian.xlsx
+++ b/PlexByte.App.MoCap.Docs/Code Dockumentation fabian.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7968" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7968" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,10 @@
     <sheet name="Expense" sheetId="2" r:id="rId3"/>
     <sheet name="Timeslice" sheetId="4" r:id="rId4"/>
     <sheet name="UIManager" sheetId="5" r:id="rId5"/>
+    <sheet name="ObjectManager" sheetId="6" r:id="rId6"/>
+    <sheet name="DataManager" sheetId="8" r:id="rId7"/>
+    <sheet name="BackendService" sheetId="9" r:id="rId8"/>
+    <sheet name="FormManager" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="248">
   <si>
     <t>Name</t>
   </si>
@@ -658,6 +662,168 @@
       </rPr>
       <t xml:space="preserve"> The selected project is not being loadet in the account panel</t>
     </r>
+  </si>
+  <si>
+    <t>UpsertProjectFromForm</t>
+  </si>
+  <si>
+    <t>This method updates or insert a project object created from the form in the DB</t>
+  </si>
+  <si>
+    <t>UpsertExpenseFromForm</t>
+  </si>
+  <si>
+    <t>UpsertTimesliceFromForm</t>
+  </si>
+  <si>
+    <t>UpsertProjectMapping</t>
+  </si>
+  <si>
+    <t>ObjectManager</t>
+  </si>
+  <si>
+    <t>The project from the form is being created and forwarded tu the dataManager</t>
+  </si>
+  <si>
+    <t>A default timeslice is being returned</t>
+  </si>
+  <si>
+    <t>A default expense is being returned</t>
+  </si>
+  <si>
+    <t>The user is being forwarded to the dataManager</t>
+  </si>
+  <si>
+    <t>GetProjectById</t>
+  </si>
+  <si>
+    <t>This method get a project based on the id specified from the database</t>
+  </si>
+  <si>
+    <t>UpsertProject</t>
+  </si>
+  <si>
+    <t>UpsertTimeslice</t>
+  </si>
+  <si>
+    <t>This method inserts or updates a project mapping in the database</t>
+  </si>
+  <si>
+    <t>This method inserts or updated a project in the database</t>
+  </si>
+  <si>
+    <t>This method inserts or updates a timeslice in the database</t>
+  </si>
+  <si>
+    <t>Gets a project from the database and creates a project object</t>
+  </si>
+  <si>
+    <t>The timeslice object is being forwarded to the backendService</t>
+  </si>
+  <si>
+    <t>The project object is being forwarded to the backendService</t>
+  </si>
+  <si>
+    <t>A project mapping is being forwarded to the backendService</t>
+  </si>
+  <si>
+    <t>DataManager</t>
+  </si>
+  <si>
+    <t>PlexByte.MoCap.WinForms</t>
+  </si>
+  <si>
+    <t>GetExpenseById</t>
+  </si>
+  <si>
+    <t>GetTimesliceById</t>
+  </si>
+  <si>
+    <t>This method gets a project by the id from the database</t>
+  </si>
+  <si>
+    <t>This method gets a timeslice by the id from the database</t>
+  </si>
+  <si>
+    <t>This method gets a expense by the id from the database</t>
+  </si>
+  <si>
+    <t>GetExpenseByProjectId</t>
+  </si>
+  <si>
+    <t>This method gets all Expenses of a project.</t>
+  </si>
+  <si>
+    <t>GetTimesliceByProjectId</t>
+  </si>
+  <si>
+    <t>This method gets all Timeslices of a project</t>
+  </si>
+  <si>
+    <t>GetAccountByProjectId</t>
+  </si>
+  <si>
+    <t>This method returns all users with TotalTime and TotalValue by projectId</t>
+  </si>
+  <si>
+    <t>InsertProject</t>
+  </si>
+  <si>
+    <t>InsertTimeslice</t>
+  </si>
+  <si>
+    <t>InsertProjectMapping</t>
+  </si>
+  <si>
+    <t>This method inserts the timeslice in the database</t>
+  </si>
+  <si>
+    <t>This method inserts the project mapping in the database</t>
+  </si>
+  <si>
+    <t>This method inserts the project in the database</t>
+  </si>
+  <si>
+    <t>The project is being returned from the id given</t>
+  </si>
+  <si>
+    <t>The timeslice is being returned from the id given</t>
+  </si>
+  <si>
+    <t>The expense is being returned from the id given</t>
+  </si>
+  <si>
+    <t>The mapping is being inserted into the database</t>
+  </si>
+  <si>
+    <t>mapping is being inserted into the database</t>
+  </si>
+  <si>
+    <t>The expenses are being returned from the projectId given</t>
+  </si>
+  <si>
+    <t>The timeslice are being returned from the projectId given</t>
+  </si>
+  <si>
+    <t>The account is being returned from the projectId given</t>
+  </si>
+  <si>
+    <t>FormManager</t>
+  </si>
+  <si>
+    <t>CreateFormFromObject</t>
+  </si>
+  <si>
+    <t>This method creates a form based on the object type and initializes its fields with the objects values</t>
+  </si>
+  <si>
+    <t>This method creates a form based on an object provided and initializes the forms values using the objects properties</t>
+  </si>
+  <si>
+    <t>Returns the object and dockContent</t>
+  </si>
+  <si>
+    <t>Opens the project panel from the object given</t>
   </si>
 </sst>
 </file>
@@ -710,7 +876,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -875,11 +1041,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -909,6 +1097,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2893,8 +3087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2918,7 +3112,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>12</v>
+        <v>216</v>
       </c>
       <c r="C2" s="7"/>
     </row>
@@ -3129,4 +3323,882 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="131.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="12"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="13"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="13"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="9"/>
+      <c r="B21" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="9"/>
+      <c r="B22" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="10"/>
+      <c r="B24" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="131.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="12"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="13"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="13"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="9"/>
+      <c r="B21" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="9"/>
+      <c r="B22" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="10"/>
+      <c r="B24" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>214</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="131.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="12"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="13"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="13"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="9"/>
+      <c r="B22" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="20"/>
+      <c r="B23" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="9"/>
+      <c r="B26" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="9"/>
+      <c r="B29" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="9"/>
+      <c r="B30" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
+      <c r="B31" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
+      <c r="B32" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+      <c r="B33" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="10"/>
+      <c r="B34" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="131.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="12"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="13"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="13"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="30"/>
+      <c r="B16" s="31" t="s">
+        <v>243</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="10"/>
+      <c r="B20" s="31" t="s">
+        <v>243</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>